<commit_message>
Add test coverage actions and some test data in 2020.05.13
</commit_message>
<xml_diff>
--- a/tests/data/PlSql2PostgreTestCase.xlsx
+++ b/tests/data/PlSql2PostgreTestCase.xlsx
@@ -1069,10 +1069,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">SET AUTOCOMMIT ON
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">set colsep ""
 </t>
   </si>
@@ -1634,11 +1630,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">/* SET AUTOCOMMIT ON */
-\set AUTOCOMMIT ON
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">/* set colsep "" */
 \pset fieldsep ""
 </t>
@@ -2000,6 +1991,17 @@
   </si>
   <si>
     <t xml:space="preserve">DROP VIEW TEST_SYM CASCADE ;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SET AUTOCOMMIT 1
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/* SET AUTOCOMMIT 1 */
+\set AUTOCOMMIT on
 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2450,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" topLeftCell="G47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2528,7 +2530,7 @@
         <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
@@ -2561,7 +2563,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>116</v>
@@ -3452,7 +3454,7 @@
         <v>162</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3476,7 +3478,7 @@
         <v>163</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3500,7 +3502,7 @@
         <v>164</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3524,7 +3526,7 @@
         <v>165</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3548,7 +3550,7 @@
         <v>166</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3572,7 +3574,7 @@
         <v>167</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3596,7 +3598,7 @@
         <v>168</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3620,7 +3622,7 @@
         <v>169</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3644,7 +3646,7 @@
         <v>170</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3668,7 +3670,7 @@
         <v>171</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -3740,7 +3742,7 @@
         <v>176</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3764,7 +3766,7 @@
         <v>177</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3788,7 +3790,7 @@
         <v>178</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3812,7 +3814,7 @@
         <v>179</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3836,7 +3838,7 @@
         <v>180</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3857,10 +3859,10 @@
         <v>60</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>181</v>
+        <v>357</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>286</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3881,10 +3883,10 @@
         <v>44</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3905,10 +3907,10 @@
         <v>19</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3929,10 +3931,10 @@
         <v>57</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3953,10 +3955,10 @@
         <v>58</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3977,10 +3979,10 @@
         <v>59</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4001,10 +4003,10 @@
         <v>60</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4025,10 +4027,10 @@
         <v>44</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4049,10 +4051,10 @@
         <v>19</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4073,10 +4075,10 @@
         <v>57</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4097,10 +4099,10 @@
         <v>58</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4121,10 +4123,10 @@
         <v>59</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4145,10 +4147,10 @@
         <v>60</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4169,10 +4171,10 @@
         <v>44</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4193,10 +4195,10 @@
         <v>19</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4217,10 +4219,10 @@
         <v>57</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4241,10 +4243,10 @@
         <v>58</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4265,10 +4267,10 @@
         <v>59</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4289,10 +4291,10 @@
         <v>60</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4313,10 +4315,10 @@
         <v>68</v>
       </c>
       <c r="F77" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="G77" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4337,10 +4339,10 @@
         <v>57</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4361,10 +4363,10 @@
         <v>58</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4385,10 +4387,10 @@
         <v>59</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4409,10 +4411,10 @@
         <v>60</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4433,10 +4435,10 @@
         <v>44</v>
       </c>
       <c r="F82" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="G82" s="14" t="s">
         <v>206</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4457,10 +4459,10 @@
         <v>19</v>
       </c>
       <c r="F83" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" s="14" t="s">
         <v>208</v>
-      </c>
-      <c r="G83" s="14" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4481,10 +4483,10 @@
         <v>79</v>
       </c>
       <c r="F84" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G84" s="14" t="s">
         <v>210</v>
-      </c>
-      <c r="G84" s="14" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4505,10 +4507,10 @@
         <v>111</v>
       </c>
       <c r="F85" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G85" s="14" t="s">
         <v>212</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4529,10 +4531,10 @@
         <v>112</v>
       </c>
       <c r="F86" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="G86" s="14" t="s">
         <v>214</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4553,10 +4555,10 @@
         <v>46</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G87" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4577,10 +4579,10 @@
         <v>46</v>
       </c>
       <c r="F88" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G88" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="G88" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4601,10 +4603,10 @@
         <v>86</v>
       </c>
       <c r="F89" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G89" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="G89" s="14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4625,10 +4627,10 @@
         <v>87</v>
       </c>
       <c r="F90" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G90" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="G90" s="14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4649,10 +4651,10 @@
         <v>88</v>
       </c>
       <c r="F91" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G91" s="14" t="s">
         <v>223</v>
-      </c>
-      <c r="G91" s="14" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4673,10 +4675,10 @@
         <v>89</v>
       </c>
       <c r="F92" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G92" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="G92" s="14" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4697,10 +4699,10 @@
         <v>90</v>
       </c>
       <c r="F93" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="G93" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4721,10 +4723,10 @@
         <v>91</v>
       </c>
       <c r="F94" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G94" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="G94" s="14" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4745,10 +4747,10 @@
         <v>46</v>
       </c>
       <c r="F95" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="G95" s="14" t="s">
         <v>231</v>
-      </c>
-      <c r="G95" s="14" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4769,10 +4771,10 @@
         <v>86</v>
       </c>
       <c r="F96" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="G96" s="14" t="s">
         <v>233</v>
-      </c>
-      <c r="G96" s="14" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4793,10 +4795,10 @@
         <v>87</v>
       </c>
       <c r="F97" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G97" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="G97" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4817,10 +4819,10 @@
         <v>88</v>
       </c>
       <c r="F98" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G98" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="G98" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4841,10 +4843,10 @@
         <v>89</v>
       </c>
       <c r="F99" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G99" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="G99" s="14" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4865,10 +4867,10 @@
         <v>90</v>
       </c>
       <c r="F100" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G100" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="G100" s="14" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4889,10 +4891,10 @@
         <v>91</v>
       </c>
       <c r="F101" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G101" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="G101" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4913,10 +4915,10 @@
         <v>46</v>
       </c>
       <c r="F102" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="G102" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="G102" s="14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4937,10 +4939,10 @@
         <v>46</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -4961,10 +4963,10 @@
         <v>46</v>
       </c>
       <c r="F104" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G104" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="G104" s="14" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -4985,10 +4987,10 @@
         <v>46</v>
       </c>
       <c r="F105" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G105" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="G105" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -5009,10 +5011,10 @@
         <v>46</v>
       </c>
       <c r="F106" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="G106" s="14" t="s">
         <v>252</v>
-      </c>
-      <c r="G106" s="14" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -5033,10 +5035,10 @@
         <v>46</v>
       </c>
       <c r="F107" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="G107" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="G107" s="14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -5057,10 +5059,10 @@
         <v>46</v>
       </c>
       <c r="F108" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G108" s="14" t="s">
         <v>256</v>
-      </c>
-      <c r="G108" s="14" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -5081,10 +5083,10 @@
         <v>46</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G109" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -5105,10 +5107,10 @@
         <v>46</v>
       </c>
       <c r="F110" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="G110" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="G110" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -5129,10 +5131,10 @@
         <v>46</v>
       </c>
       <c r="F111" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="G111" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="G111" s="14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="108" x14ac:dyDescent="0.15">
@@ -5153,10 +5155,10 @@
         <v>46</v>
       </c>
       <c r="F112" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="G112" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="G112" s="14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="108" x14ac:dyDescent="0.15">
@@ -5177,10 +5179,10 @@
         <v>46</v>
       </c>
       <c r="F113" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G113" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="G113" s="14" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -5201,10 +5203,10 @@
         <v>46</v>
       </c>
       <c r="F114" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="G114" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="G114" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -5225,10 +5227,10 @@
         <v>46</v>
       </c>
       <c r="F115" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G115" s="14" t="s">
         <v>269</v>
-      </c>
-      <c r="G115" s="14" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="135" x14ac:dyDescent="0.15">
@@ -5249,10 +5251,10 @@
         <v>46</v>
       </c>
       <c r="F116" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="G116" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="G116" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="135" x14ac:dyDescent="0.15">
@@ -5273,10 +5275,10 @@
         <v>46</v>
       </c>
       <c r="F117" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="G117" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="G117" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5297,10 +5299,10 @@
         <v>44</v>
       </c>
       <c r="F118" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="G118" s="14" t="s">
         <v>314</v>
-      </c>
-      <c r="G118" s="14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5321,10 +5323,10 @@
         <v>19</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G119" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5345,10 +5347,10 @@
         <v>44</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5369,10 +5371,10 @@
         <v>19</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5393,10 +5395,10 @@
         <v>44</v>
       </c>
       <c r="F122" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G122" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5417,10 +5419,10 @@
         <v>19</v>
       </c>
       <c r="F123" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G123" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5432,19 +5434,19 @@
         <v>106</v>
       </c>
       <c r="C124" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D124" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="F124" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G124" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="G124" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5456,19 +5458,19 @@
         <v>106</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D125" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="F125" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G125" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5480,19 +5482,19 @@
         <v>106</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D126" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F126" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G126" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5504,19 +5506,19 @@
         <v>106</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F127" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G127" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5528,19 +5530,19 @@
         <v>106</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D128" s="16" t="s">
         <v>109</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F128" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G128" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5552,19 +5554,19 @@
         <v>106</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D129" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F129" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="E129" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F129" s="14" t="s">
-        <v>337</v>
-      </c>
       <c r="G129" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5573,22 +5575,22 @@
         <v>129</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C130" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="E130" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D130" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="F130" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G130" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="G130" s="14" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5597,22 +5599,22 @@
         <v>130</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F131" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G131" s="14" t="s">
         <v>342</v>
-      </c>
-      <c r="G131" s="14" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5621,10 +5623,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D132" s="16" t="s">
         <v>99</v>
@@ -5633,10 +5635,10 @@
         <v>44</v>
       </c>
       <c r="F132" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G132" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5645,10 +5647,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>99</v>
@@ -5657,10 +5659,10 @@
         <v>19</v>
       </c>
       <c r="F133" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G133" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5669,10 +5671,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D134" s="16" t="s">
         <v>109</v>
@@ -5681,10 +5683,10 @@
         <v>44</v>
       </c>
       <c r="F134" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="G134" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="G134" s="14" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5693,22 +5695,22 @@
         <v>134</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F135" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G135" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5717,22 +5719,22 @@
         <v>135</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F136" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G136" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="G136" s="14" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -5741,22 +5743,22 @@
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F137" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="G137" s="14" t="s">
         <v>356</v>
-      </c>
-      <c r="G137" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some functions in 2020.05.14
</commit_message>
<xml_diff>
--- a/tests/data/PlSql2PostgreTestCase.xlsx
+++ b/tests/data/PlSql2PostgreTestCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="374">
   <si>
     <t>項番</t>
     <rPh sb="0" eb="1">
@@ -2002,6 +2002,86 @@
   <si>
     <t xml:space="preserve">/* SET AUTOCOMMIT 1 */
 \set AUTOCOMMIT on
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>削除</t>
+    <rPh sb="0" eb="2">
+      <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小文字</t>
+    <rPh sb="0" eb="3">
+      <t>コモジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大文字</t>
+    <rPh sb="0" eb="3">
+      <t>オオモジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop function test_user.test_function;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">drop function test_user.test_function() CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP FUNCTION TEST_USER.TEST_FUNCTION;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DROP FUNCTION TEST_USER.TEST_FUNCTION() CASCADE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>修正</t>
+    <rPh sb="0" eb="2">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">alter function test_func compile;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/* alter function test_func compile; */
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTER FUNCTION TEST_FUNC COMPLIE;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/* ALTER FUNCTION TEST_FUNC COMPLIE; */
 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2126,7 +2206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2146,6 +2226,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2450,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="F127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5379,7 +5464,7 @@
     </row>
     <row r="122" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
-        <f t="shared" ref="A122:A137" si="2">ROW()-1</f>
+        <f t="shared" ref="A122:A141" si="2">ROW()-1</f>
         <v>121</v>
       </c>
       <c r="B122" s="7" t="s">
@@ -5759,6 +5844,102 @@
       </c>
       <c r="G137" s="14" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A138" s="2">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="B138" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="D138" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="E138" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="F138" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G138" s="14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A139" s="2">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="B139" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="D139" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="E139" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="F139" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G139" s="14" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A140" s="2">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="B140" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="D140" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="E140" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="F140" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G140" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A141" s="2">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="B141" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="C141" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="D141" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="E141" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="F141" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G141" s="14" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>